<commit_message>
select for linking those not linked
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2237,6 +2237,50 @@
         </is>
       </c>
     </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Zwane deserved a fair chance as Chiefs coach – Mabedi</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Zwane</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Q4800783</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>South African footballer</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>President Mnangagwa officiates 4th ZNDU graduation ceremony</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>President Mnangagwa</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Q510523</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>President of the Republic of Zimbabwe</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>